<commit_message>
conditional formatting on "percent funded"
</commit_message>
<xml_diff>
--- a/Starter/CrowdfundingBook.xlsx
+++ b/Starter/CrowdfundingBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Desktop\2023Bootcamp_Classwork\excel-challenge\Starter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CDEF7B-3445-469F-AAA8-85CC5B3E9C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13CDAD5-4D63-41BF-91AD-AA9F5744D25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27855" yWindow="180" windowWidth="27810" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6661,7 +6661,71 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -7013,7 +7077,7 @@
   <dimension ref="A1:O1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -55076,17 +55140,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"live"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"canceled"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"successful"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FFC00000"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>